<commit_message>
organize the files and add the AI
</commit_message>
<xml_diff>
--- a/backend/data/الغزوات.xlsx
+++ b/backend/data/الغزوات.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f58b35e40015d4ae/سطح المكتب/university/8Summer Training/Raya.github.io/backend/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f58b35e40015d4ae/سطح المكتب/university/8Summer Training/Raya.github.io/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="488" documentId="11_B8ACEE991895064A1CB304B4C4E8A0A449CCCB21" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CAB52D86-2B97-43BF-8A40-38EB23C63707}"/>
+  <xr:revisionPtr revIDLastSave="499" documentId="11_B8ACEE991895064A1CB304B4C4E8A0A449CCCB21" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0EE66978-B70A-43A5-BD36-69D2B3CEE940}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3152,7 +3152,7 @@
   <dimension ref="A1:AD1033"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A104" sqref="A104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4113,7 +4113,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:30" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="24" t="s">
         <v>145</v>
       </c>
@@ -5025,7 +5025,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="38" spans="1:30" ht="175" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:30" ht="175" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
         <v>287</v>
       </c>
@@ -5346,7 +5346,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="44" spans="1:30" ht="125" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:30" ht="125" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
         <v>336</v>
       </c>
@@ -5552,7 +5552,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="48" spans="1:30" ht="237.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:30" ht="237.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
         <v>373</v>
       </c>
@@ -7071,7 +7071,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="77" spans="1:30" ht="100" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:30" ht="100" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="21" t="s">
         <v>590</v>
       </c>
@@ -8338,7 +8338,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="102" spans="1:30" ht="137.5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:30" ht="137.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="20" t="s">
         <v>781</v>
       </c>
@@ -8436,7 +8436,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="104" spans="1:30" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:30" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A104" s="20" t="s">
         <v>794</v>
       </c>
@@ -10383,12 +10383,7 @@
   <autoFilter ref="A1:O1033" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="0">
       <filters>
-        <filter val="الغزوات البحرية الإسلامية على جزر المتوسط"/>
-        <filter val="غزوة بني المصطلق (غزوة المريسيع)"/>
-        <filter val="فتح المدائن"/>
-        <filter val="معركة الثني, المذار"/>
-        <filter val="معركة المذار والحيرة"/>
-        <filter val="معركة المصيخ"/>
+        <filter val="حملة خرسان الثانية"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>